<commit_message>
swap friedrichs and kilians part
</commit_message>
<xml_diff>
--- a/401/data/zeeman/zeeman.xlsx
+++ b/401/data/zeeman/zeeman.xlsx
@@ -1863,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AP104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AP104" sqref="AP104"/>
+    <sheetView tabSelected="1" topLeftCell="AH86" workbookViewId="0">
+      <selection activeCell="AM95" sqref="AM95:AM104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15446,16 +15446,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK95">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f>(-7.31668+6.19432)/(8.7-6)*(8.7-6)-6.19432</f>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL95">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f>(152.451-132.452)/(8.7-6)*(8.7-6)+132.452</f>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM95">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f>(-141.396+41.5064)/(8.7-6)*(8.7-6)-41.5604</f>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN95" s="1">
         <f t="shared" si="56"/>
@@ -15467,7 +15467,7 @@
       </c>
       <c r="AP95" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="96" spans="3:42" x14ac:dyDescent="0.25">
@@ -15598,16 +15598,16 @@
         <v>9.8204747492036298E-26</v>
       </c>
       <c r="AK96">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" ref="AK96:AK104" si="67">(-7.31668+6.19432)/(8.7-6)*(8.7-6)-6.19432</f>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL96">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" ref="AL96:AL104" si="68">(152.451-132.452)/(8.7-6)*(8.7-6)+132.452</f>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM96">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" ref="AM96:AM104" si="69">(-141.396+41.5064)/(8.7-6)*(8.7-6)-41.5604</f>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN96" s="1">
         <f t="shared" si="56"/>
@@ -15619,7 +15619,7 @@
       </c>
       <c r="AP96" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="97" spans="3:42" x14ac:dyDescent="0.25">
@@ -15744,16 +15744,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK97">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL97">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM97">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN97" s="1">
         <f t="shared" si="56"/>
@@ -15765,7 +15765,7 @@
       </c>
       <c r="AP97" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="98" spans="3:42" x14ac:dyDescent="0.25">
@@ -15890,16 +15890,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK98">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL98">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM98">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN98" s="1">
         <f t="shared" si="56"/>
@@ -15911,7 +15911,7 @@
       </c>
       <c r="AP98" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="99" spans="3:42" x14ac:dyDescent="0.25">
@@ -16040,16 +16040,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK99">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL99">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM99">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN99" s="1">
         <f t="shared" si="56"/>
@@ -16061,7 +16061,7 @@
       </c>
       <c r="AP99" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="100" spans="3:42" x14ac:dyDescent="0.25">
@@ -16190,16 +16190,16 @@
         <v>-8.2407951876757583E-26</v>
       </c>
       <c r="AK100">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL100">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM100">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN100" s="1">
         <f t="shared" si="56"/>
@@ -16211,7 +16211,7 @@
       </c>
       <c r="AP100" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="101" spans="3:42" x14ac:dyDescent="0.25">
@@ -16336,16 +16336,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK101">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL101">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM101">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN101" s="1">
         <f t="shared" si="56"/>
@@ -16357,7 +16357,7 @@
       </c>
       <c r="AP101" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="102" spans="3:42" x14ac:dyDescent="0.25">
@@ -16482,16 +16482,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK102">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL102">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM102">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN102" s="1">
         <f t="shared" si="56"/>
@@ -16503,7 +16503,7 @@
       </c>
       <c r="AP102" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="103" spans="3:42" x14ac:dyDescent="0.25">
@@ -16634,16 +16634,16 @@
         <v>-1.1568084751271028E-25</v>
       </c>
       <c r="AK103">
-        <f t="shared" si="43"/>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL103">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM103">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN103" s="1">
         <f t="shared" si="56"/>
@@ -16655,7 +16655,7 @@
       </c>
       <c r="AP103" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
     <row r="104" spans="3:42" x14ac:dyDescent="0.25">
@@ -16780,16 +16780,16 @@
         <v>#VALUE!</v>
       </c>
       <c r="AK104">
-        <f>(-7.31668+6.19432)/(8.7-6)*(N104-6)-6.19432</f>
-        <v>-7.2335422222222228</v>
+        <f t="shared" si="67"/>
+        <v>-7.3166799999999999</v>
       </c>
       <c r="AL104">
-        <f t="shared" si="54"/>
-        <v>150.96959259259259</v>
+        <f t="shared" si="68"/>
+        <v>152.45099999999999</v>
       </c>
       <c r="AM104">
-        <f t="shared" si="55"/>
-        <v>-134.0507703703704</v>
+        <f t="shared" si="69"/>
+        <v>-141.44999999999999</v>
       </c>
       <c r="AN104" s="1">
         <f t="shared" si="56"/>
@@ -16801,7 +16801,7 @@
       </c>
       <c r="AP104" s="1">
         <f t="shared" si="58"/>
-        <v>0.62656734111111101</v>
+        <v>0.62575336999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>